<commit_message>
Support local pgs catalogs
</commit_message>
<xml_diff>
--- a/tests/data/metadata.xlsx
+++ b/tests/data/metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukfor/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukfor/Development/git/nf-pgs/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBF69F1-D5B3-D943-BCA5-B52C65EC2522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FB4400-394D-FC4C-B51D-2F4BCDCA54A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6760" yWindow="820" windowWidth="31040" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,20 +40,20 @@
     <t>hg19</t>
   </si>
   <si>
-    <t>http://ftp.ebi.ac.uk/pub/databases/spot/pgs/scores/PGS000001/ScoringFiles/PGS000001.txt.gz</t>
-  </si>
-  <si>
-    <t>Wu et al. - 2021 </t>
-  </si>
-  <si>
     <t>IBK000001</t>
+  </si>
+  <si>
+    <t>IBK000001.txt.gz</t>
+  </si>
+  <si>
+    <t>Copy of PGS000001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,13 +68,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,22 +102,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,7 +451,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -495,25 +482,22 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>5114</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>